<commit_message>
corrected the coordinates for player and robot
</commit_message>
<xml_diff>
--- a/sampleAIOutput.xlsx
+++ b/sampleAIOutput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TdrDi\Documents\GitHub\Badmintobot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9FA399-6828-42BF-B6B8-019B85DCA801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616127B3-2448-4BBA-8871-A0EC6DD7E4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -368,7 +368,7 @@
   <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -392,13 +392,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1393.8969999999999</v>
+        <v>-538.96999999999935</v>
       </c>
       <c r="C2">
-        <v>9.4749999999999996</v>
+        <v>94.75</v>
       </c>
       <c r="D2">
-        <v>95.420000000000016</v>
+        <v>954.20000000000016</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -407,13 +407,13 @@
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="B3">
-        <v>1303.664</v>
+        <v>363.36000000000013</v>
       </c>
       <c r="C3">
-        <v>15.621</v>
+        <v>156.21</v>
       </c>
       <c r="D3">
-        <v>139.10300000000001</v>
+        <v>1391.0300000000002</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -422,13 +422,13 @@
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="B4">
-        <v>1203.884</v>
+        <v>1361.1599999999999</v>
       </c>
       <c r="C4">
-        <v>16.106999999999999</v>
+        <v>161.07</v>
       </c>
       <c r="D4">
-        <v>192.32400000000001</v>
+        <v>1923.2400000000002</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -437,13 +437,13 @@
         <v>0.1</v>
       </c>
       <c r="B5">
-        <v>1121.394</v>
+        <v>2186.06</v>
       </c>
       <c r="C5">
-        <v>15.987</v>
+        <v>159.87</v>
       </c>
       <c r="D5">
-        <v>233.71699999999998</v>
+        <v>2337.17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -452,13 +452,13 @@
         <v>0.13333333333333333</v>
       </c>
       <c r="B6">
-        <v>1046.8420000000001</v>
+        <v>2931.579999999999</v>
       </c>
       <c r="C6">
-        <v>18.757000000000001</v>
+        <v>187.57000000000002</v>
       </c>
       <c r="D6">
-        <v>271.97000000000003</v>
+        <v>2719.7000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -467,13 +467,13 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="B7">
-        <v>981.58100000000002</v>
+        <v>3584.1899999999996</v>
       </c>
       <c r="C7">
-        <v>20.751000000000001</v>
+        <v>207.51000000000002</v>
       </c>
       <c r="D7">
-        <v>304.06799999999998</v>
+        <v>3040.68</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -482,13 +482,13 @@
         <v>0.19999999999999998</v>
       </c>
       <c r="B8">
-        <v>929.25</v>
+        <v>4107.5</v>
       </c>
       <c r="C8">
-        <v>22.518000000000001</v>
+        <v>225.18</v>
       </c>
       <c r="D8">
-        <v>328.07000000000005</v>
+        <v>3280.7000000000007</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -497,13 +497,13 @@
         <v>0.23333333333333331</v>
       </c>
       <c r="B9">
-        <v>883.21500000000003</v>
+        <v>4567.8499999999995</v>
       </c>
       <c r="C9">
-        <v>23.911999999999999</v>
+        <v>239.12</v>
       </c>
       <c r="D9">
-        <v>349.76599999999996</v>
+        <v>3497.66</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -512,13 +512,13 @@
         <v>0.26666666666666666</v>
       </c>
       <c r="B10">
-        <v>836.24099999999999</v>
+        <v>5037.59</v>
       </c>
       <c r="C10">
-        <v>24.678999999999998</v>
+        <v>246.79</v>
       </c>
       <c r="D10">
-        <v>370.65800000000002</v>
+        <v>3706.58</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -527,13 +527,13 @@
         <v>0.3</v>
       </c>
       <c r="B11">
-        <v>793.71900000000005</v>
+        <v>5462.8099999999995</v>
       </c>
       <c r="C11">
-        <v>27.065999999999999</v>
+        <v>270.65999999999997</v>
       </c>
       <c r="D11">
-        <v>388.83699999999999</v>
+        <v>3888.37</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -542,13 +542,13 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="B12">
-        <v>756.33299999999997</v>
+        <v>5836.67</v>
       </c>
       <c r="C12">
-        <v>28.335999999999999</v>
+        <v>283.36</v>
       </c>
       <c r="D12">
-        <v>403.60900000000004</v>
+        <v>4036.09</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -557,13 +557,13 @@
         <v>0.36666666666666664</v>
       </c>
       <c r="B13">
-        <v>722.94799999999998</v>
+        <v>6170.52</v>
       </c>
       <c r="C13">
-        <v>28.777000000000001</v>
+        <v>287.77</v>
       </c>
       <c r="D13">
-        <v>415.71600000000001</v>
+        <v>4157.16</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -572,13 +572,13 @@
         <v>0.39999999999999997</v>
       </c>
       <c r="B14">
-        <v>692.03599999999994</v>
+        <v>6479.64</v>
       </c>
       <c r="C14">
-        <v>30.305</v>
+        <v>303.05</v>
       </c>
       <c r="D14">
-        <v>426.97400000000005</v>
+        <v>4269.7400000000007</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -587,13 +587,13 @@
         <v>0.43333333333333329</v>
       </c>
       <c r="B15">
-        <v>656.94100000000003</v>
+        <v>6830.59</v>
       </c>
       <c r="C15">
-        <v>31.95</v>
+        <v>319.5</v>
       </c>
       <c r="D15">
-        <v>437.42499999999995</v>
+        <v>4374.25</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -602,13 +602,13 @@
         <v>0.46666666666666662</v>
       </c>
       <c r="B16">
-        <v>621.10400000000004</v>
+        <v>7188.9599999999991</v>
       </c>
       <c r="C16">
-        <v>32.865000000000002</v>
+        <v>328.65000000000003</v>
       </c>
       <c r="D16">
-        <v>448.68799999999999</v>
+        <v>4486.88</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -617,13 +617,13 @@
         <v>0.49999999999999994</v>
       </c>
       <c r="B17">
-        <v>582.57799999999997</v>
+        <v>7574.22</v>
       </c>
       <c r="C17">
-        <v>33.841999999999999</v>
+        <v>338.41999999999996</v>
       </c>
       <c r="D17">
-        <v>460.86599999999999</v>
+        <v>4608.66</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -632,13 +632,13 @@
         <v>0.53333333333333333</v>
       </c>
       <c r="B18">
-        <v>550.16499999999996</v>
+        <v>7898.35</v>
       </c>
       <c r="C18">
-        <v>34.640999999999998</v>
+        <v>346.40999999999997</v>
       </c>
       <c r="D18">
-        <v>468.9</v>
+        <v>4689</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -647,13 +647,13 @@
         <v>0.56666666666666665</v>
       </c>
       <c r="B19">
-        <v>536.98400000000004</v>
+        <v>8030.16</v>
       </c>
       <c r="C19">
-        <v>35.823</v>
+        <v>358.23</v>
       </c>
       <c r="D19">
-        <v>467.29200000000003</v>
+        <v>4672.92</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -662,13 +662,13 @@
         <v>0.6</v>
       </c>
       <c r="B20">
-        <v>521.73400000000004</v>
+        <v>8182.66</v>
       </c>
       <c r="C20">
-        <v>37.933</v>
+        <v>379.33</v>
       </c>
       <c r="D20">
-        <v>464.59500000000003</v>
+        <v>4645.9500000000007</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -677,13 +677,13 @@
         <v>0.6333333333333333</v>
       </c>
       <c r="B21">
-        <v>485.71499999999992</v>
+        <v>8542.85</v>
       </c>
       <c r="C21">
-        <v>38.884999999999998</v>
+        <v>388.84999999999997</v>
       </c>
       <c r="D21">
-        <v>472.33199999999999</v>
+        <v>4723.32</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -692,13 +692,13 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="B22">
-        <v>466.05700000000002</v>
+        <v>8739.43</v>
       </c>
       <c r="C22">
-        <v>39.853999999999999</v>
+        <v>398.53999999999996</v>
       </c>
       <c r="D22">
-        <v>473.74300000000005</v>
+        <v>4737.43</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -707,13 +707,13 @@
         <v>0.7</v>
       </c>
       <c r="B23">
-        <v>433.08999999999992</v>
+        <v>9069.1</v>
       </c>
       <c r="C23">
-        <v>41.2</v>
+        <v>412</v>
       </c>
       <c r="D23">
-        <v>478.65599999999995</v>
+        <v>4786.5599999999995</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -722,13 +722,13 @@
         <v>0.73333333333333328</v>
       </c>
       <c r="B24">
-        <v>420.02</v>
+        <v>9199.7999999999993</v>
       </c>
       <c r="C24">
-        <v>41.945999999999998</v>
+        <v>419.46</v>
       </c>
       <c r="D24">
-        <v>473.30899999999997</v>
+        <v>4733.09</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -737,13 +737,13 @@
         <v>0.76666666666666661</v>
       </c>
       <c r="B25">
-        <v>397.92100000000005</v>
+        <v>9420.7899999999991</v>
       </c>
       <c r="C25">
-        <v>44.93</v>
+        <v>449.3</v>
       </c>
       <c r="D25">
-        <v>473.01199999999994</v>
+        <v>4730.119999999999</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -752,13 +752,13 @@
         <v>0.79999999999999993</v>
       </c>
       <c r="B26">
-        <v>372.05899999999997</v>
+        <v>9679.41</v>
       </c>
       <c r="C26">
-        <v>45.122</v>
+        <v>451.22</v>
       </c>
       <c r="D26">
-        <v>469.83500000000004</v>
+        <v>4698.3500000000004</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -767,13 +767,13 @@
         <v>0.83333333333333326</v>
       </c>
       <c r="B27">
-        <v>353.45900000000006</v>
+        <v>9865.41</v>
       </c>
       <c r="C27">
-        <v>45.594999999999999</v>
+        <v>455.95</v>
       </c>
       <c r="D27">
-        <v>466.822</v>
+        <v>4668.22</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -782,13 +782,13 @@
         <v>0.86666666666666659</v>
       </c>
       <c r="B28">
-        <v>347.19299999999998</v>
+        <v>9928.07</v>
       </c>
       <c r="C28">
-        <v>46.670999999999999</v>
+        <v>466.71</v>
       </c>
       <c r="D28">
-        <v>457.78499999999997</v>
+        <v>4577.8499999999995</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -797,13 +797,13 @@
         <v>0.89999999999999991</v>
       </c>
       <c r="B29">
-        <v>327.44399999999996</v>
+        <v>10125.560000000001</v>
       </c>
       <c r="C29">
-        <v>49.165999999999997</v>
+        <v>491.65999999999997</v>
       </c>
       <c r="D29">
-        <v>452.77099999999996</v>
+        <v>4527.7099999999991</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -812,13 +812,13 @@
         <v>0.93333333333333324</v>
       </c>
       <c r="B30">
-        <v>314.00500000000011</v>
+        <v>10259.949999999999</v>
       </c>
       <c r="C30">
-        <v>48.978999999999999</v>
+        <v>489.78999999999996</v>
       </c>
       <c r="D30">
-        <v>444.90800000000002</v>
+        <v>4449.08</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -827,13 +827,13 @@
         <v>0.96666666666666656</v>
       </c>
       <c r="B31">
-        <v>292.51700000000005</v>
+        <v>10474.83</v>
       </c>
       <c r="C31">
-        <v>50.545999999999999</v>
+        <v>505.46</v>
       </c>
       <c r="D31">
-        <v>439.56600000000003</v>
+        <v>4395.66</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -842,13 +842,13 @@
         <v>0.99999999999999989</v>
       </c>
       <c r="B32">
-        <v>290.97299999999996</v>
+        <v>10490.27</v>
       </c>
       <c r="C32">
-        <v>52.963999999999999</v>
+        <v>529.64</v>
       </c>
       <c r="D32">
-        <v>424.60699999999997</v>
+        <v>4246.07</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -857,13 +857,13 @@
         <v>1.0333333333333332</v>
       </c>
       <c r="B33">
-        <v>250.44900000000007</v>
+        <v>10895.509999999998</v>
       </c>
       <c r="C33">
-        <v>53.728000000000002</v>
+        <v>537.28</v>
       </c>
       <c r="D33">
-        <v>427.11400000000003</v>
+        <v>4271.1400000000003</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -872,13 +872,13 @@
         <v>1.0666666666666667</v>
       </c>
       <c r="B34">
-        <v>232.49499999999989</v>
+        <v>11075.050000000001</v>
       </c>
       <c r="C34">
-        <v>53.631</v>
+        <v>536.30999999999995</v>
       </c>
       <c r="D34">
-        <v>417.39499999999998</v>
+        <v>4173.95</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -887,13 +887,13 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B35">
-        <v>216.57199999999989</v>
+        <v>11234.28</v>
       </c>
       <c r="C35">
-        <v>56.624000000000002</v>
+        <v>566.24</v>
       </c>
       <c r="D35">
-        <v>407.83900000000006</v>
+        <v>4078.3900000000003</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -902,13 +902,13 @@
         <v>1.1333333333333335</v>
       </c>
       <c r="B36">
-        <v>200.55700000000002</v>
+        <v>11394.43</v>
       </c>
       <c r="C36">
-        <v>57.537999999999997</v>
+        <v>575.38</v>
       </c>
       <c r="D36">
-        <v>397.03599999999994</v>
+        <v>3970.3599999999997</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -917,13 +917,13 @@
         <v>1.166666666666667</v>
       </c>
       <c r="B37">
-        <v>199.48199999999997</v>
+        <v>11405.18</v>
       </c>
       <c r="C37">
-        <v>56.88</v>
+        <v>568.80000000000007</v>
       </c>
       <c r="D37">
-        <v>382.69100000000003</v>
+        <v>3826.9100000000003</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -932,13 +932,13 @@
         <v>1.2000000000000004</v>
       </c>
       <c r="B38">
-        <v>182.05300000000011</v>
+        <v>11579.47</v>
       </c>
       <c r="C38">
-        <v>58.883000000000003</v>
+        <v>588.83000000000004</v>
       </c>
       <c r="D38">
-        <v>371.60599999999999</v>
+        <v>3716.06</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -947,13 +947,13 @@
         <v>1.2333333333333338</v>
       </c>
       <c r="B39">
-        <v>164.40000000000009</v>
+        <v>11756</v>
       </c>
       <c r="C39">
-        <v>60.914000000000001</v>
+        <v>609.14</v>
       </c>
       <c r="D39">
-        <v>360.92600000000004</v>
+        <v>3609.26</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -962,13 +962,13 @@
         <v>1.2666666666666673</v>
       </c>
       <c r="B40">
-        <v>148.48900000000003</v>
+        <v>11915.11</v>
       </c>
       <c r="C40">
-        <v>61.850999999999999</v>
+        <v>618.51</v>
       </c>
       <c r="D40">
-        <v>350.05700000000002</v>
+        <v>3500.57</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -977,13 +977,13 @@
         <v>1.3000000000000007</v>
       </c>
       <c r="B41">
-        <v>129.23199999999997</v>
+        <v>12107.68</v>
       </c>
       <c r="C41">
-        <v>62.856000000000002</v>
+        <v>628.56000000000006</v>
       </c>
       <c r="D41">
-        <v>335.64</v>
+        <v>3356.3999999999996</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -992,13 +992,13 @@
         <v>1.3333333333333341</v>
       </c>
       <c r="B42">
-        <v>133.07400000000007</v>
+        <v>12069.259999999998</v>
       </c>
       <c r="C42">
-        <v>64.593999999999994</v>
+        <v>645.93999999999994</v>
       </c>
       <c r="D42">
-        <v>315.666</v>
+        <v>3156.66</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1007,13 +1007,13 @@
         <v>1.3666666666666676</v>
       </c>
       <c r="B43">
-        <v>124.92499999999995</v>
+        <v>12150.75</v>
       </c>
       <c r="C43">
-        <v>65.77</v>
+        <v>657.69999999999993</v>
       </c>
       <c r="D43">
-        <v>301.85000000000002</v>
+        <v>3018.5</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1022,13 +1022,13 @@
         <v>1.400000000000001</v>
       </c>
       <c r="B44">
-        <v>97.430000000000064</v>
+        <v>12425.699999999999</v>
       </c>
       <c r="C44">
-        <v>66.584000000000003</v>
+        <v>665.84</v>
       </c>
       <c r="D44">
-        <v>289.77499999999998</v>
+        <v>2897.75</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1037,13 +1037,13 @@
         <v>1.4333333333333345</v>
       </c>
       <c r="B45">
-        <v>86.564000000000078</v>
+        <v>12534.359999999999</v>
       </c>
       <c r="C45">
-        <v>67.837000000000003</v>
+        <v>678.37</v>
       </c>
       <c r="D45">
-        <v>274.29899999999998</v>
+        <v>2742.99</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1052,13 +1052,13 @@
         <v>1.4666666666666679</v>
       </c>
       <c r="B46">
-        <v>66.631000000000085</v>
+        <v>12733.689999999999</v>
       </c>
       <c r="C46">
-        <v>69.983000000000004</v>
+        <v>699.83</v>
       </c>
       <c r="D46">
-        <v>259.82100000000003</v>
+        <v>2598.21</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1067,13 +1067,13 @@
         <v>1.5000000000000013</v>
       </c>
       <c r="B47">
-        <v>72.433999999999969</v>
+        <v>12675.66</v>
       </c>
       <c r="C47">
-        <v>70.561000000000007</v>
+        <v>705.61000000000013</v>
       </c>
       <c r="D47">
-        <v>240.495</v>
+        <v>2404.9499999999998</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1082,13 +1082,13 @@
         <v>1.5333333333333348</v>
       </c>
       <c r="B48">
-        <v>42.628999999999905</v>
+        <v>12973.710000000001</v>
       </c>
       <c r="C48">
-        <v>72.572000000000003</v>
+        <v>725.72</v>
       </c>
       <c r="D48">
-        <v>227.36799999999999</v>
+        <v>2273.6799999999998</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1097,13 +1097,13 @@
         <v>1.5666666666666682</v>
       </c>
       <c r="B49">
-        <v>39.739000000000033</v>
+        <v>13002.61</v>
       </c>
       <c r="C49">
-        <v>71.837000000000003</v>
+        <v>718.37</v>
       </c>
       <c r="D49">
-        <v>206.899</v>
+        <v>2068.9899999999998</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1112,13 +1112,13 @@
         <v>1.6000000000000016</v>
       </c>
       <c r="B50">
-        <v>45.701999999999998</v>
+        <v>12942.98</v>
       </c>
       <c r="C50">
-        <v>73.472999999999999</v>
+        <v>734.73</v>
       </c>
       <c r="D50">
-        <v>188.10399999999998</v>
+        <v>1881.04</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1127,13 +1127,13 @@
         <v>1.6333333333333351</v>
       </c>
       <c r="B51">
-        <v>40.69399999999996</v>
+        <v>12993.060000000001</v>
       </c>
       <c r="C51">
-        <v>73.897000000000006</v>
+        <v>738.97</v>
       </c>
       <c r="D51">
-        <v>168.988</v>
+        <v>1689.88</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1142,13 +1142,13 @@
         <v>1.6666666666666685</v>
       </c>
       <c r="B52">
-        <v>29.273999999999887</v>
+        <v>13107.260000000002</v>
       </c>
       <c r="C52">
-        <v>74.085999999999999</v>
+        <v>740.86</v>
       </c>
       <c r="D52">
-        <v>152.55399999999997</v>
+        <v>1525.5399999999997</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1157,13 +1157,13 @@
         <v>1.700000000000002</v>
       </c>
       <c r="B53">
-        <v>39.869999999999891</v>
+        <v>13001.300000000001</v>
       </c>
       <c r="C53">
-        <v>74.864000000000004</v>
+        <v>748.64</v>
       </c>
       <c r="D53">
-        <v>128.26999999999998</v>
+        <v>1282.6999999999998</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1172,13 +1172,13 @@
         <v>1.7333333333333354</v>
       </c>
       <c r="B54">
-        <v>28.638999999999896</v>
+        <v>13113.61</v>
       </c>
       <c r="C54">
-        <v>75.036000000000001</v>
+        <v>750.36</v>
       </c>
       <c r="D54">
-        <v>110.99299999999999</v>
+        <v>1109.9299999999998</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1187,13 +1187,13 @@
         <v>1.7666666666666688</v>
       </c>
       <c r="B55">
-        <v>8.25</v>
+        <v>13317.5</v>
       </c>
       <c r="C55">
-        <v>76.103999999999999</v>
+        <v>761.04</v>
       </c>
       <c r="D55">
-        <v>93.348000000000013</v>
+        <v>933.48000000000013</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1202,13 +1202,13 @@
         <v>1.8000000000000023</v>
       </c>
       <c r="B56">
-        <v>-3.2729999999999109</v>
+        <v>13432.73</v>
       </c>
       <c r="C56">
-        <v>78.421999999999997</v>
+        <v>784.22</v>
       </c>
       <c r="D56">
-        <v>76.446000000000026</v>
+        <v>764.46000000000026</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1217,13 +1217,13 @@
         <v>1.8333333333333357</v>
       </c>
       <c r="B57">
-        <v>18.124000000000024</v>
+        <v>13218.76</v>
       </c>
       <c r="C57">
-        <v>77.141000000000005</v>
+        <v>771.41000000000008</v>
       </c>
       <c r="D57">
-        <v>54.187000000000012</v>
+        <v>541.87000000000012</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1232,13 +1232,13 @@
         <v>1.8666666666666691</v>
       </c>
       <c r="B58">
-        <v>-5.3179999999999836</v>
+        <v>13453.18</v>
       </c>
       <c r="C58">
-        <v>79.322999999999993</v>
+        <v>793.2299999999999</v>
       </c>
       <c r="D58">
-        <v>32.402999999999992</v>
+        <v>324.02999999999992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>